<commit_message>
Section 3: Course + Exercises
</commit_message>
<xml_diff>
--- a/Excel_Homework_Exercises.xlsx
+++ b/Excel_Homework_Exercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Knowledge Database\Excel\Excel Homework Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF47496-0EEC-4E00-9C29-46EDD48ED092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F402069-5663-4527-AA83-866629977C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="709" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7246,7 +7246,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7292,10 +7292,22 @@
       <c r="C2" s="2">
         <v>90</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
+      <c r="D2" s="43" t="str">
+        <f>IF(C2&gt;=60, "PASS", "FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="E2" s="43" t="str">
+        <f>IF(C2&gt;=90, "A", IF(C2&gt;=80, "B", IF(C2&gt;=70, "C", IF(C2 &gt;=60, "D", "F"))))</f>
+        <v>A</v>
+      </c>
+      <c r="F2" s="43" t="str">
+        <f>IF(OR(C2&lt;60, C2&gt;90), "Outlier", "Avg")</f>
+        <v>Avg</v>
+      </c>
+      <c r="G2" s="43" t="str">
+        <f>IF(AND(B2="M",C2&gt;95), "Male Achiever", IF(AND(B2="F",C2&gt;95),"Female Achiever", "None"))</f>
+        <v>None</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -7307,10 +7319,22 @@
       <c r="C3" s="2">
         <v>80</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
+      <c r="D3" s="43" t="str">
+        <f t="shared" ref="D3:D16" si="0">IF(C3&gt;=60, "PASS", "FAIL")</f>
+        <v>PASS</v>
+      </c>
+      <c r="E3" s="43" t="str">
+        <f t="shared" ref="E3:E16" si="1">IF(C3&gt;=90, "A", IF(C3&gt;=80, "B", IF(C3&gt;=70, "C", IF(C3 &gt;=60, "D", "F"))))</f>
+        <v>B</v>
+      </c>
+      <c r="F3" s="43" t="str">
+        <f t="shared" ref="F3:F16" si="2">IF(OR(C3&lt;60, C3&gt;90), "Outlier", "Avg")</f>
+        <v>Avg</v>
+      </c>
+      <c r="G3" s="43" t="str">
+        <f t="shared" ref="G3:G16" si="3">IF(AND(B3="M",C3&gt;95), "Male Achiever", IF(AND(B3="F",C3&gt;95),"Female Achiever", "None"))</f>
+        <v>None</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -7322,10 +7346,22 @@
       <c r="C4" s="2">
         <v>96</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="D4" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E4" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+      <c r="F4" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Outlier</v>
+      </c>
+      <c r="G4" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>Female Achiever</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -7337,10 +7373,22 @@
       <c r="C5" s="2">
         <v>72</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
+      <c r="D5" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E5" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="F5" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Avg</v>
+      </c>
+      <c r="G5" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>None</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -7352,10 +7400,22 @@
       <c r="C6" s="2">
         <v>69</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
+      <c r="D6" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E6" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>D</v>
+      </c>
+      <c r="F6" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Avg</v>
+      </c>
+      <c r="G6" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>None</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -7367,10 +7427,22 @@
       <c r="C7" s="2">
         <v>52</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
+      <c r="D7" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+      <c r="E7" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="F7" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Outlier</v>
+      </c>
+      <c r="G7" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>None</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -7382,10 +7454,22 @@
       <c r="C8" s="2">
         <v>99</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
+      <c r="D8" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E8" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+      <c r="F8" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Outlier</v>
+      </c>
+      <c r="G8" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>Male Achiever</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -7397,10 +7481,22 @@
       <c r="C9" s="2">
         <v>82</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
+      <c r="D9" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E9" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+      <c r="F9" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Avg</v>
+      </c>
+      <c r="G9" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>None</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -7412,10 +7508,22 @@
       <c r="C10" s="2">
         <v>67</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
+      <c r="D10" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E10" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>D</v>
+      </c>
+      <c r="F10" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Avg</v>
+      </c>
+      <c r="G10" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>None</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -7427,10 +7535,22 @@
       <c r="C11" s="2">
         <v>90</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
+      <c r="D11" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E11" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+      <c r="F11" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Avg</v>
+      </c>
+      <c r="G11" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>None</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -7442,10 +7562,22 @@
       <c r="C12" s="2">
         <v>83</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="D12" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E12" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+      <c r="F12" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Avg</v>
+      </c>
+      <c r="G12" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>None</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -7457,10 +7589,22 @@
       <c r="C13" s="2">
         <v>89</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
+      <c r="D13" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E13" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+      <c r="F13" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Avg</v>
+      </c>
+      <c r="G13" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>None</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -7472,10 +7616,22 @@
       <c r="C14" s="2">
         <v>60</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="D14" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E14" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>D</v>
+      </c>
+      <c r="F14" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Avg</v>
+      </c>
+      <c r="G14" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>None</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -7487,10 +7643,22 @@
       <c r="C15" s="2">
         <v>63</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
+      <c r="D15" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E15" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>D</v>
+      </c>
+      <c r="F15" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Avg</v>
+      </c>
+      <c r="G15" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>None</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -7502,10 +7670,22 @@
       <c r="C16" s="2">
         <v>59</v>
       </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
+      <c r="D16" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>FAIL</v>
+      </c>
+      <c r="E16" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="F16" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Outlier</v>
+      </c>
+      <c r="G16" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v>None</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Section4: Course + Homework
</commit_message>
<xml_diff>
--- a/Excel_Homework_Exercises.xlsx
+++ b/Excel_Homework_Exercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Knowledge Database\Excel\Excel Homework Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F402069-5663-4527-AA83-866629977C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9A87D0-E056-48EA-9F3A-FCE54B64CC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="709" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="27000" windowHeight="14235" tabRatio="709" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulas 101" sheetId="19" r:id="rId1"/>
@@ -7245,7 +7245,7 @@
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -7700,7 +7700,9 @@
   </sheetPr>
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7825,7 +7827,10 @@
       <c r="E5" s="8">
         <v>3072</v>
       </c>
-      <c r="H5" s="36"/>
+      <c r="H5" s="36">
+        <f>SUMIF($A:$A,$H$2,$D:$D)</f>
+        <v>620</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -7889,9 +7894,18 @@
       <c r="G8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H8" s="36"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="36"/>
+      <c r="H8" s="36">
+        <f>SUMIFS($D:$D,$A:$A,$H$2,$C:$C,G8)</f>
+        <v>166</v>
+      </c>
+      <c r="I8" s="46">
+        <f>SUMIFS($E:$E,$A:$A,$H$2,$C:$C,G8)</f>
+        <v>10015</v>
+      </c>
+      <c r="J8" s="36">
+        <f>COUNTIFS($A:$A,$H$2,$C:$C,$G8)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -7912,9 +7926,18 @@
       <c r="G9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="36"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="36"/>
+      <c r="H9" s="36">
+        <f>SUMIFS($D:$D,$A:$A,$H$2,$C:$C,G9)</f>
+        <v>372</v>
+      </c>
+      <c r="I9" s="46">
+        <f>SUMIFS($E:$E,$A:$A,$H$2,$C:$C,G9)</f>
+        <v>42628</v>
+      </c>
+      <c r="J9" s="36">
+        <f>COUNTIFS($A:$A,$H$2,$C:$C,$G9)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -7935,9 +7958,18 @@
       <c r="G10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="36"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="36"/>
+      <c r="H10" s="36">
+        <f>SUMIFS($D:$D,$A:$A,$H$2,$C:$C,G10)</f>
+        <v>82</v>
+      </c>
+      <c r="I10" s="46">
+        <f>SUMIFS($E:$E,$A:$A,$H$2,$C:$C,G10)</f>
+        <v>6300</v>
+      </c>
+      <c r="J10" s="36">
+        <f>COUNTIFS($A:$A,$H$2,$C:$C,$G10)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">

</xml_diff>